<commit_message>
Performance improvements by faster mem zeroing
The main difference of `ConcurrentVec` from more performant `ConcurrentBag` is due to the fact that `ConcurrentVec` zeroes out new positions upon each new allocation. This is a requirement to provide safe versions of the `get` and `iter` methods; in other words, to allow safe concurrent read and write opeations.

In the prior version, memory zeroing had been handled by the concurrent bag's fill strategy which requires iteration over the new allocated positions.

In the new version. a memory zeroing concurrent bag is wrapped which now directly uses `PinnedVec`s `grow_to` method to zero out the memory on allocation. The implementations often reduce to a memset call and hence provides performance improvements.

Benchmarks are repeated, expected improvements are observed and reported.
</commit_message>
<xml_diff>
--- a/benches/results/collect.xlsx
+++ b/benches/results/collect.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\uurdev\orx\orx-concurrent-vec\benches\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18BA38F-0407-43DF-9A9F-EA33539DE94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B0BAC2-CAB4-4597-B9E6-043FED94896E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3885" yWindow="1635" windowWidth="21165" windowHeight="19170" xr2:uid="{201707E4-C870-4993-88CE-4A7BD9846E2B}"/>
+    <workbookView xWindow="3885" yWindow="1635" windowWidth="21165" windowHeight="19170" activeTab="1" xr2:uid="{201707E4-C870-4993-88CE-4A7BD9846E2B}"/>
   </bookViews>
   <sheets>
     <sheet name="collect_with_push" sheetId="5" r:id="rId1"/>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7FC78D-902C-4DF1-8F50-38A3D8921053}">
   <dimension ref="B1:I41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C20:C21"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,10 +765,12 @@
         <v>0</v>
       </c>
       <c r="E2">
+        <f>collect_with_extend!E2</f>
         <v>0.26207999999999998</v>
       </c>
       <c r="G2" s="22">
-        <v>18.701000000000001</v>
+        <f>collect_with_extend!G2</f>
+        <v>19.791</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -785,7 +787,7 @@
         <v>4.7229000000000001</v>
       </c>
       <c r="G3" s="22">
-        <v>20.556000000000001</v>
+        <v>18.974</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -799,10 +801,10 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>5.6811999999999996</v>
+        <v>4.4450000000000003</v>
       </c>
       <c r="G4" s="22">
-        <v>13.717000000000001</v>
+        <v>14.282999999999999</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -816,11 +818,11 @@
         <v>0</v>
       </c>
       <c r="E5" s="20">
-        <v>4.0445000000000002</v>
+        <v>4.1616</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="23">
-        <v>12.634</v>
+        <v>12.961</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
@@ -893,10 +895,12 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>1.2151000000000001</v>
+        <f>collect_with_extend!E10</f>
+        <v>1.3241000000000001</v>
       </c>
       <c r="G10" s="22">
-        <v>87.033000000000001</v>
+        <f>collect_with_extend!G10</f>
+        <v>81.653999999999996</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -914,7 +918,7 @@
         <v>22.34</v>
       </c>
       <c r="G11" s="22">
-        <v>93.644000000000005</v>
+        <v>82.436999999999998</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -929,10 +933,10 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>20.074999999999999</v>
+        <v>20.071000000000002</v>
       </c>
       <c r="G12" s="22">
-        <v>66.125</v>
+        <v>65.004000000000005</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -947,11 +951,11 @@
         <v>0</v>
       </c>
       <c r="E13" s="20">
-        <v>19.478999999999999</v>
+        <v>19.440999999999999</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="20">
-        <v>47.485999999999997</v>
+        <v>48.92</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
@@ -1056,7 +1060,7 @@
       </c>
       <c r="G26" s="8">
         <f t="shared" ref="G26:G41" si="4">G2</f>
-        <v>18.701000000000001</v>
+        <v>19.791</v>
       </c>
       <c r="H26" s="5">
         <f>G26/G$26</f>
@@ -1086,11 +1090,11 @@
       </c>
       <c r="G27" s="18">
         <f t="shared" si="4"/>
-        <v>20.556000000000001</v>
+        <v>18.974</v>
       </c>
       <c r="H27" s="19">
         <f t="shared" ref="H27:H29" si="8">G27/G$26</f>
-        <v>1.0991925565477783</v>
+        <v>0.95871860946895049</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1108,19 +1112,19 @@
       </c>
       <c r="E28" s="18">
         <f t="shared" si="3"/>
-        <v>5.6811999999999996</v>
+        <v>4.4450000000000003</v>
       </c>
       <c r="F28" s="19">
         <f t="shared" si="7"/>
-        <v>21.677350427350426</v>
+        <v>16.960470085470089</v>
       </c>
       <c r="G28" s="18">
         <f t="shared" si="4"/>
-        <v>13.717000000000001</v>
+        <v>14.282999999999999</v>
       </c>
       <c r="H28" s="19">
         <f t="shared" si="8"/>
-        <v>0.7334901876904979</v>
+        <v>0.72169167803547063</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1138,19 +1142,19 @@
       </c>
       <c r="E29" s="9">
         <f t="shared" si="3"/>
-        <v>4.0445000000000002</v>
+        <v>4.1616</v>
       </c>
       <c r="F29" s="7">
         <f t="shared" si="7"/>
-        <v>15.432310744810747</v>
+        <v>15.87912087912088</v>
       </c>
       <c r="G29" s="9">
         <f t="shared" si="4"/>
-        <v>12.634</v>
+        <v>12.961</v>
       </c>
       <c r="H29" s="7">
         <f t="shared" si="8"/>
-        <v>0.67557884605101326</v>
+        <v>0.65489363852256077</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1288,7 +1292,7 @@
       </c>
       <c r="E34" s="8">
         <f t="shared" si="3"/>
-        <v>1.2151000000000001</v>
+        <v>1.3241000000000001</v>
       </c>
       <c r="F34" s="5">
         <f>E34/E$34</f>
@@ -1296,7 +1300,7 @@
       </c>
       <c r="G34" s="8">
         <f t="shared" si="4"/>
-        <v>87.033000000000001</v>
+        <v>81.653999999999996</v>
       </c>
       <c r="H34" s="5">
         <f>G34/G$34</f>
@@ -1322,15 +1326,15 @@
       </c>
       <c r="F35" s="19">
         <f t="shared" ref="F35:F37" si="11">E35/E$34</f>
-        <v>18.385318080816393</v>
+        <v>16.871837474510986</v>
       </c>
       <c r="G35" s="18">
         <f t="shared" si="4"/>
-        <v>93.644000000000005</v>
+        <v>82.436999999999998</v>
       </c>
       <c r="H35" s="19">
         <f t="shared" ref="H35:H37" si="12">G35/G$34</f>
-        <v>1.0759596934496112</v>
+        <v>1.009589242413109</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1348,19 +1352,19 @@
       </c>
       <c r="E36" s="18">
         <f t="shared" si="3"/>
-        <v>20.074999999999999</v>
+        <v>20.071000000000002</v>
       </c>
       <c r="F36" s="19">
         <f t="shared" si="11"/>
-        <v>16.521273969220641</v>
+        <v>15.158220678196511</v>
       </c>
       <c r="G36" s="18">
         <f t="shared" si="4"/>
-        <v>66.125</v>
+        <v>65.004000000000005</v>
       </c>
       <c r="H36" s="19">
         <f t="shared" si="12"/>
-        <v>0.75976928291567569</v>
+        <v>0.79609082224998173</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1378,19 +1382,19 @@
       </c>
       <c r="E37" s="9">
         <f t="shared" si="3"/>
-        <v>19.478999999999999</v>
+        <v>19.440999999999999</v>
       </c>
       <c r="F37" s="7">
         <f t="shared" si="11"/>
-        <v>16.030779359723478</v>
+        <v>14.682425798655689</v>
       </c>
       <c r="G37" s="9">
         <f t="shared" si="4"/>
-        <v>47.485999999999997</v>
+        <v>48.92</v>
       </c>
       <c r="H37" s="7">
         <f t="shared" si="12"/>
-        <v>0.54560913676421585</v>
+        <v>0.59911333186371774</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1733,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAC745C-D468-49EC-93AB-3CA0AF648CD4}">
   <dimension ref="B1:I41"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,10 +1792,10 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.94308000000000003</v>
+        <v>0.59357000000000004</v>
       </c>
       <c r="G3" s="22">
-        <v>17.271999999999998</v>
+        <v>16.343</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -1805,10 +1809,10 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.95247000000000004</v>
+        <v>0.35904999999999998</v>
       </c>
       <c r="G4" s="22">
-        <v>18.001000000000001</v>
+        <v>9.4992000000000001</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -1822,11 +1826,11 @@
         <v>0</v>
       </c>
       <c r="E5" s="20">
-        <v>0.92379999999999995</v>
+        <v>0.34448000000000001</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="23">
-        <v>17.175999999999998</v>
+        <v>6.4676</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
@@ -1917,10 +1921,10 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>3.9298000000000002</v>
+        <v>2.1206999999999998</v>
       </c>
       <c r="G11" s="22">
-        <v>75.006</v>
+        <v>64.709000000000003</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -1935,10 +1939,10 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>3.89425</v>
+        <v>1.0075000000000001</v>
       </c>
       <c r="G12" s="22">
-        <v>75.548000000000002</v>
+        <v>41.076999999999998</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -1953,11 +1957,11 @@
         <v>0</v>
       </c>
       <c r="E13" s="20">
-        <v>3.4870000000000001</v>
+        <v>1.0028999999999999</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="20">
-        <v>75.346580000000003</v>
+        <v>26.298999999999999</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
@@ -2084,19 +2088,19 @@
       </c>
       <c r="E27" s="18">
         <f t="shared" si="1"/>
-        <v>0.94308000000000003</v>
+        <v>0.59357000000000004</v>
       </c>
       <c r="F27" s="19">
         <f t="shared" ref="F27:F29" si="4">E27/E$26</f>
-        <v>3.598443223443224</v>
+        <v>2.2648427960927964</v>
       </c>
       <c r="G27" s="18">
         <f t="shared" si="2"/>
-        <v>17.271999999999998</v>
+        <v>16.343</v>
       </c>
       <c r="H27" s="19">
         <f t="shared" ref="H27:H29" si="5">G27/G$26</f>
-        <v>0.87271992319741287</v>
+        <v>0.82577939467434691</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2114,19 +2118,19 @@
       </c>
       <c r="E28" s="18">
         <f t="shared" si="1"/>
-        <v>0.95247000000000004</v>
+        <v>0.35904999999999998</v>
       </c>
       <c r="F28" s="19">
         <f t="shared" si="4"/>
-        <v>3.6342719780219785</v>
+        <v>1.3700015262515264</v>
       </c>
       <c r="G28" s="18">
         <f t="shared" si="2"/>
-        <v>18.001000000000001</v>
+        <v>9.4992000000000001</v>
       </c>
       <c r="H28" s="19">
         <f t="shared" si="5"/>
-        <v>0.90955484816330656</v>
+        <v>0.4799757465514628</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2144,19 +2148,19 @@
       </c>
       <c r="E29" s="9">
         <f t="shared" si="1"/>
-        <v>0.92379999999999995</v>
+        <v>0.34448000000000001</v>
       </c>
       <c r="F29" s="7">
         <f t="shared" si="4"/>
-        <v>3.5248778998778998</v>
+        <v>1.3144078144078146</v>
       </c>
       <c r="G29" s="9">
         <f t="shared" si="2"/>
-        <v>17.175999999999998</v>
+        <v>6.4676</v>
       </c>
       <c r="H29" s="7">
         <f t="shared" si="5"/>
-        <v>0.86786923348997014</v>
+        <v>0.32679500783184273</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2324,19 +2328,19 @@
       </c>
       <c r="E35" s="18">
         <f t="shared" si="1"/>
-        <v>3.9298000000000002</v>
+        <v>2.1206999999999998</v>
       </c>
       <c r="F35" s="19">
         <f t="shared" ref="F35:F37" si="8">E35/E$34</f>
-        <v>2.9679027263801827</v>
+        <v>1.6016161921305034</v>
       </c>
       <c r="G35" s="18">
         <f t="shared" si="2"/>
-        <v>75.006</v>
+        <v>64.709000000000003</v>
       </c>
       <c r="H35" s="19">
         <f t="shared" ref="H35:H37" si="9">G35/G$34</f>
-        <v>0.91858329046954224</v>
+        <v>0.79247801699855491</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2354,19 +2358,19 @@
       </c>
       <c r="E36" s="18">
         <f t="shared" si="1"/>
-        <v>3.89425</v>
+        <v>1.0075000000000001</v>
       </c>
       <c r="F36" s="19">
         <f t="shared" si="8"/>
-        <v>2.941054301034665</v>
+        <v>0.76089419228154975</v>
       </c>
       <c r="G36" s="18">
         <f t="shared" si="2"/>
-        <v>75.548000000000002</v>
+        <v>41.076999999999998</v>
       </c>
       <c r="H36" s="19">
         <f t="shared" si="9"/>
-        <v>0.92522105469419758</v>
+        <v>0.50306169936561584</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2384,19 +2388,19 @@
       </c>
       <c r="E37" s="9">
         <f t="shared" si="1"/>
-        <v>3.4870000000000001</v>
+        <v>1.0028999999999999</v>
       </c>
       <c r="F37" s="7">
         <f t="shared" si="8"/>
-        <v>2.6334868967600635</v>
+        <v>0.75742013443093414</v>
       </c>
       <c r="G37" s="9">
         <f t="shared" si="2"/>
-        <v>75.346580000000003</v>
+        <v>26.298999999999999</v>
       </c>
       <c r="H37" s="7">
         <f t="shared" si="9"/>
-        <v>0.92275430474930809</v>
+        <v>0.32207852646532931</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>